<commit_message>
Plan logique version 1.0 avec erreur
</commit_message>
<xml_diff>
--- a/Planning des matchs.xlsx
+++ b/Planning des matchs.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\remip\Documents\GitHub\UE2-Projet-r-seau\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maxim\OneDrive\Documents\GitHub\UE2-Projet-r-seau\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="2" documentId="59E93DB6715E9A230005B2392F5AD1F3923E04E0" xr6:coauthVersionLast="25" xr6:coauthVersionMax="25" xr10:uidLastSave="{ED979F64-5C36-4BFE-85D4-677706C7B6F9}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5628" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="66">
   <si>
     <t>Jour 1</t>
   </si>
@@ -218,13 +219,7 @@
     <t>00h</t>
   </si>
   <si>
-    <t>00h30</t>
-  </si>
-  <si>
     <t>Remise des Prix</t>
-  </si>
-  <si>
-    <t>Cérémonie de cloture</t>
   </si>
   <si>
     <t>Cérémonie d'ouverture</t>
@@ -233,7 +228,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -440,29 +435,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
@@ -483,6 +460,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -490,6 +476,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -805,11 +800,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:P33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32:N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -830,7 +825,7 @@
       </c>
     </row>
     <row r="2" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="B2" s="18" t="s">
+      <c r="B2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="5" t="s">
@@ -842,13 +837,13 @@
       <c r="E2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="12" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="5" t="s">
@@ -860,7 +855,7 @@
       <c r="L2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="19" t="s">
+      <c r="M2" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N2" s="5" t="s">
@@ -871,13 +866,13 @@
       <c r="B3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="16"/>
-      <c r="E3" s="16"/>
-      <c r="F3" s="16"/>
-      <c r="G3" s="17"/>
+      <c r="C3" s="32" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="33"/>
+      <c r="E3" s="33"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="34"/>
       <c r="I3" s="2" t="s">
         <v>7</v>
       </c>
@@ -891,7 +886,7 @@
       <c r="M3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="19" t="s">
         <v>52</v>
       </c>
     </row>
@@ -899,11 +894,11 @@
       <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="40"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="37"/>
       <c r="I4" s="4" t="s">
         <v>8</v>
       </c>
@@ -923,7 +918,7 @@
       <c r="D5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="20" t="s">
+      <c r="E5" s="14" t="s">
         <v>14</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -940,10 +935,10 @@
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
       <c r="N5" s="6"/>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="P5" s="11" t="s">
         <v>60</v>
       </c>
     </row>
@@ -953,7 +948,7 @@
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="12"/>
+      <c r="E6" s="10"/>
       <c r="F6" s="4"/>
       <c r="G6" s="6"/>
       <c r="I6" s="4" t="s">
@@ -968,14 +963,14 @@
       <c r="L6" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="M6" s="27" t="s">
+      <c r="M6" s="21" t="s">
         <v>48</v>
       </c>
       <c r="N6" s="6"/>
-      <c r="O6" s="30" t="s">
+      <c r="O6" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="31" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1023,7 +1018,7 @@
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-      <c r="N8" s="11"/>
+      <c r="N8" s="9"/>
     </row>
     <row r="9" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B9" s="4" t="s">
@@ -1031,7 +1026,7 @@
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="23" t="s">
         <v>16</v>
       </c>
       <c r="F9" s="4"/>
@@ -1039,13 +1034,13 @@
       <c r="I9" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="15" t="s">
+      <c r="J9" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="17"/>
+      <c r="K9" s="33"/>
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="34"/>
     </row>
     <row r="10" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B10" s="4" t="s">
@@ -1053,60 +1048,60 @@
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="12"/>
+      <c r="E10" s="10"/>
       <c r="F10" s="4"/>
       <c r="G10" s="6"/>
       <c r="I10" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="7"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="8"/>
-      <c r="M10" s="8"/>
-      <c r="N10" s="14"/>
+      <c r="J10" s="38"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="39"/>
+      <c r="M10" s="39"/>
+      <c r="N10" s="40"/>
     </row>
     <row r="11" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="16"/>
-      <c r="E11" s="16"/>
-      <c r="F11" s="16"/>
-      <c r="G11" s="17"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="34"/>
       <c r="I11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J11" s="38"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="39"/>
-      <c r="M11" s="39"/>
-      <c r="N11" s="40"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="36"/>
+      <c r="L11" s="36"/>
+      <c r="M11" s="36"/>
+      <c r="N11" s="37"/>
     </row>
     <row r="12" spans="2:16" x14ac:dyDescent="0.3">
       <c r="B12" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="38"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
-      <c r="G12" s="40"/>
+      <c r="C12" s="35"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="37"/>
       <c r="I12" s="4" t="s">
         <v>19</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="K12" s="25" t="s">
+      <c r="K12" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="L12" s="13" t="s">
+      <c r="L12" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="M12" s="29" t="s">
+      <c r="M12" s="23" t="s">
         <v>53</v>
       </c>
       <c r="N12" s="6"/>
@@ -1121,7 +1116,7 @@
       <c r="D13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="20" t="s">
+      <c r="E13" s="14" t="s">
         <v>37</v>
       </c>
       <c r="F13" s="4" t="s">
@@ -1143,13 +1138,13 @@
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="12"/>
+      <c r="E14" s="10"/>
       <c r="F14" s="4"/>
       <c r="G14" s="3"/>
       <c r="I14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="J14" s="28"/>
+      <c r="J14" s="22"/>
       <c r="K14" s="3"/>
       <c r="L14" s="6"/>
       <c r="M14" s="4"/>
@@ -1169,7 +1164,7 @@
       <c r="I15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="J15" s="18" t="s">
         <v>49</v>
       </c>
       <c r="K15" s="4" t="s">
@@ -1183,13 +1178,13 @@
       <c r="B16" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="18" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="14" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1211,7 +1206,7 @@
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="12"/>
+      <c r="E17" s="10"/>
       <c r="F17" s="4"/>
       <c r="G17" s="6"/>
       <c r="I17" s="4" t="s">
@@ -1219,7 +1214,7 @@
       </c>
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
-      <c r="L17" s="12"/>
+      <c r="L17" s="10"/>
       <c r="M17" s="4"/>
       <c r="N17" s="6"/>
     </row>
@@ -1229,17 +1224,17 @@
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
-      <c r="E18" s="10"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="3"/>
-      <c r="G18" s="11"/>
+      <c r="G18" s="9"/>
       <c r="I18" s="4" t="s">
         <v>25</v>
       </c>
       <c r="J18" s="4"/>
-      <c r="K18" s="35" t="s">
+      <c r="K18" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="L18" s="36" t="s">
+      <c r="L18" s="30" t="s">
         <v>54</v>
       </c>
       <c r="M18" s="4"/>
@@ -1249,36 +1244,36 @@
       <c r="B19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="32" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="17"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="34"/>
       <c r="I19" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="J19" s="34"/>
-      <c r="K19" s="22"/>
-      <c r="L19" s="34"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="22"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="16"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="28"/>
+      <c r="N19" s="16"/>
     </row>
     <row r="20" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B20" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="39"/>
-      <c r="E20" s="39"/>
-      <c r="F20" s="39"/>
-      <c r="G20" s="40"/>
+      <c r="C20" s="35"/>
+      <c r="D20" s="36"/>
+      <c r="E20" s="36"/>
+      <c r="F20" s="36"/>
+      <c r="G20" s="37"/>
       <c r="I20" s="4" t="s">
         <v>27</v>
       </c>
       <c r="J20" s="3"/>
-      <c r="K20" s="11"/>
+      <c r="K20" s="9"/>
       <c r="L20" s="3"/>
       <c r="M20" s="3"/>
       <c r="N20" s="6"/>
@@ -1293,7 +1288,7 @@
       <c r="D21" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E21" s="26" t="s">
+      <c r="E21" s="20" t="s">
         <v>35</v>
       </c>
       <c r="F21" s="4" t="s">
@@ -1305,12 +1300,12 @@
       <c r="I21" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="35" t="s">
+      <c r="J21" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="K21" s="24"/>
+      <c r="K21" s="18"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="36" t="s">
+      <c r="M21" s="30" t="s">
         <v>54</v>
       </c>
       <c r="N21" s="6"/>
@@ -1321,7 +1316,7 @@
       </c>
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="12"/>
+      <c r="E22" s="10"/>
       <c r="F22" s="4"/>
       <c r="G22" s="6"/>
       <c r="I22" s="4" t="s">
@@ -1339,9 +1334,9 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="8"/>
       <c r="F23" s="3"/>
-      <c r="G23" s="11"/>
+      <c r="G23" s="9"/>
       <c r="I23" s="4" t="s">
         <v>30</v>
       </c>
@@ -1355,136 +1350,132 @@
       <c r="B24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="15" t="s">
+      <c r="C24" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="17"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="34"/>
       <c r="I24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J24" s="31"/>
-      <c r="K24" s="33" t="s">
+      <c r="J24" s="25"/>
+      <c r="K24" s="27" t="s">
         <v>50</v>
       </c>
-      <c r="L24" s="21"/>
-      <c r="M24" s="21"/>
-      <c r="N24" s="22"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="16"/>
     </row>
     <row r="25" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="14"/>
+      <c r="C25" s="38"/>
+      <c r="D25" s="39"/>
+      <c r="E25" s="39"/>
+      <c r="F25" s="39"/>
+      <c r="G25" s="40"/>
       <c r="I25" s="4" t="s">
         <v>32</v>
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="6"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="12"/>
+      <c r="L25" s="10"/>
+      <c r="M25" s="10"/>
       <c r="N25" s="6"/>
     </row>
     <row r="26" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="38"/>
-      <c r="D26" s="39"/>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
-      <c r="G26" s="40"/>
+      <c r="C26" s="35"/>
+      <c r="D26" s="36"/>
+      <c r="E26" s="36"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="37"/>
       <c r="I26" s="4" t="s">
         <v>33</v>
       </c>
       <c r="J26" s="3"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="12"/>
+      <c r="K26" s="9"/>
+      <c r="L26" s="10"/>
+      <c r="M26" s="10"/>
       <c r="N26" s="6"/>
     </row>
     <row r="27" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I27" s="23" t="s">
+      <c r="I27" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="J27" s="32" t="s">
+      <c r="J27" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="K27" s="13"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="12"/>
+      <c r="K27" s="11"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="10"/>
       <c r="N27" s="6"/>
     </row>
     <row r="28" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I28" s="23" t="s">
+      <c r="I28" s="17" t="s">
         <v>46</v>
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="6"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="12"/>
+      <c r="L28" s="10"/>
+      <c r="M28" s="10"/>
       <c r="N28" s="6"/>
     </row>
     <row r="29" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I29" s="23" t="s">
+      <c r="I29" s="17" t="s">
         <v>47</v>
       </c>
       <c r="J29" s="3"/>
-      <c r="K29" s="11"/>
+      <c r="K29" s="9"/>
       <c r="L29" s="1"/>
       <c r="M29" s="1"/>
-      <c r="N29" s="11"/>
+      <c r="N29" s="9"/>
     </row>
     <row r="30" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="J30" s="15" t="s">
-        <v>65</v>
-      </c>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="17"/>
+      <c r="J30" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="K30" s="33"/>
+      <c r="L30" s="33"/>
+      <c r="M30" s="33"/>
+      <c r="N30" s="34"/>
     </row>
     <row r="31" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I31" s="23" t="s">
+      <c r="I31" s="17" t="s">
         <v>62</v>
       </c>
-      <c r="J31" s="38"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="39"/>
-      <c r="M31" s="39"/>
-      <c r="N31" s="40"/>
-      <c r="O31" s="12"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="36"/>
+      <c r="L31" s="36"/>
+      <c r="M31" s="36"/>
+      <c r="N31" s="37"/>
+      <c r="O31" s="10"/>
     </row>
     <row r="32" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="I32" s="23" t="s">
+      <c r="I32" s="17" t="s">
         <v>63</v>
       </c>
-      <c r="J32" s="15" t="s">
-        <v>66</v>
-      </c>
-      <c r="K32" s="16"/>
-      <c r="L32" s="16"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="17"/>
+      <c r="J32" s="32"/>
+      <c r="K32" s="33"/>
+      <c r="L32" s="33"/>
+      <c r="M32" s="33"/>
+      <c r="N32" s="34"/>
     </row>
     <row r="33" spans="9:14" x14ac:dyDescent="0.3">
-      <c r="I33" s="30" t="s">
-        <v>64</v>
-      </c>
-      <c r="J33" s="38"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="39"/>
-      <c r="M33" s="39"/>
-      <c r="N33" s="40"/>
+      <c r="I33" s="24"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="36"/>
+      <c r="L33" s="36"/>
+      <c r="M33" s="36"/>
+      <c r="N33" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>